<commit_message>
Changed cell D5 'City area change (sq km)' to 'City area change (hectares)'
</commit_message>
<xml_diff>
--- a/LDMP/data/summary_table_urban.xlsx
+++ b/LDMP/data/summary_table_urban.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvol\Code\LandDegradation\trends.earth\LDMP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/CI/TrendsEarth/trends.earth/LDMP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF07D82A-F505-4C92-A117-AEEB8A7F673B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80970863-1497-F244-9B86-BDE736B16FA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5963" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDG 11.3.1 Summary Table" sheetId="1" r:id="rId1"/>
@@ -104,10 +104,6 @@
     <t>City population growth rate</t>
   </si>
   <si>
-    <t>City area change
-(sq km)</t>
-  </si>
-  <si>
     <t>Population (number of people) by year</t>
   </si>
   <si>
@@ -127,6 +123,10 @@
   <si>
     <t>Total area
 of city:</t>
+  </si>
+  <si>
+    <t>City area change
+(hectares)</t>
   </si>
 </sst>
 </file>
@@ -1946,20 +1946,20 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A5:XFD6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.19921875" style="7" customWidth="1"/>
-    <col min="3" max="6" width="21.19921875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="11.53125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.19921875" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="9.19921875" style="7"/>
+    <col min="2" max="2" width="21.1640625" style="7" customWidth="1"/>
+    <col min="3" max="6" width="21.1640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1969,10 +1969,10 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>4</v>
       </c>
@@ -1982,8 +1982,8 @@
       <c r="E3" s="44"/>
       <c r="F3" s="44"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>9</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E5" s="28" t="s">
         <v>10</v>
@@ -2003,7 +2003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="16"/>
@@ -2086,7 +2086,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -2094,7 +2094,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
@@ -2102,7 +2102,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -2110,7 +2110,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
@@ -2118,7 +2118,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -2126,7 +2126,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
@@ -2134,7 +2134,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -2142,7 +2142,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -2150,7 +2150,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -2158,12 +2158,12 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="51"/>
       <c r="C20" s="52"/>
@@ -2171,13 +2171,13 @@
       <c r="E20" s="52"/>
       <c r="F20" s="52"/>
     </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:8" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="38"/>
       <c r="B22" s="23">
         <v>2000</v>
@@ -2192,10 +2192,10 @@
         <v>2015</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="37" t="s">
         <v>11</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="37" t="s">
         <v>12</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="37" t="s">
         <v>13</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="37" t="s">
         <v>14</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="37" t="s">
         <v>15</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="37" t="s">
         <v>16</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="37" t="s">
         <v>17</v>
       </c>
@@ -2279,9 +2279,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
@@ -2291,7 +2291,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37" t="s">
         <v>18</v>
       </c>
@@ -2303,9 +2303,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="36">
         <f>SUMIF($F$23:$F$31,"Yes",B23:B31)</f>
@@ -2326,13 +2326,13 @@
       <c r="F32" s="20"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B33" s="10"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" s="19" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B34" s="54"/>
       <c r="C34" s="55"/>
@@ -2341,7 +2341,7 @@
       <c r="F34" s="55"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" s="19" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
       <c r="C35" s="5"/>
@@ -2350,7 +2350,7 @@
       <c r="F35" s="20"/>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="23">
         <v>2000</v>
       </c>
@@ -2366,7 +2366,7 @@
       <c r="F36" s="20"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="37" t="s">
         <v>11</v>
       </c>
@@ -2377,7 +2377,7 @@
       <c r="F37" s="20"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="37" t="s">
         <v>12</v>
       </c>
@@ -2388,7 +2388,7 @@
       <c r="F38" s="20"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="37" t="s">
         <v>13</v>
       </c>
@@ -2399,7 +2399,7 @@
       <c r="F39" s="20"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="37" t="s">
         <v>14</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="F40" s="20"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="37" t="s">
         <v>15</v>
       </c>
@@ -2421,7 +2421,7 @@
       <c r="F41" s="20"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="37" t="s">
         <v>16</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="F42" s="20"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="37" t="s">
         <v>17</v>
       </c>
@@ -2443,9 +2443,9 @@
       <c r="F43" s="20"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B44" s="31"/>
       <c r="C44" s="31"/>
@@ -2454,7 +2454,7 @@
       <c r="F44" s="20"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="37" t="s">
         <v>18</v>
       </c>
@@ -2465,9 +2465,9 @@
       <c r="F45" s="20"/>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" s="19" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B46" s="35">
         <f>SUMIF($F$23:$F$31,"Yes",B37:B45)</f>
@@ -2488,7 +2488,7 @@
       <c r="F46" s="20"/>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
@@ -2496,7 +2496,7 @@
       <c r="F47" s="20"/>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>0</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="E48" s="47"/>
       <c r="F48" s="47"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
       <c r="B49" s="46"/>
       <c r="C49" s="47"/>
@@ -2514,13 +2514,13 @@
       <c r="E49" s="47"/>
       <c r="F49" s="47"/>
     </row>
-    <row r="50" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="45" t="s">
         <v>1</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="E51" s="49"/>
       <c r="F51" s="49"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="45" t="s">
         <v>2</v>
       </c>

</xml_diff>